<commit_message>
FIXED FILE, THIS HAS CONTENT
</commit_message>
<xml_diff>
--- a/db-first in excel.xlsx
+++ b/db-first in excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>NOT NULL</t>
-  </si>
-  <si>
-    <t>INDEX</t>
   </si>
   <si>
     <t>Modello</t>
@@ -176,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -188,24 +185,14 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="9"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
       <b val="1"/>
       <sz val="10"/>
-      <color indexed="9"/>
+      <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="9"/>
+      <color indexed="8"/>
       <name val="Helvetica Neue Medium"/>
     </font>
   </fonts>
@@ -218,24 +205,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="8"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -245,81 +232,37 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -328,92 +271,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -422,58 +280,58 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -482,10 +340,70 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -494,13 +412,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -509,13 +427,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -524,13 +442,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -539,63 +457,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,13 +475,13 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,105 +490,66 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -726,73 +558,34 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -811,11 +604,10 @@
       <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="fffefffe"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="fffefffe"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff434443"/>
       <rgbColor rgb="ffafafaf"/>
-      <rgbColor rgb="ff434443"/>
       <rgbColor rgb="ffb5b5b5"/>
       <rgbColor rgb="ff2c2c2c"/>
     </indexedColors>
@@ -834,10 +626,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="A7A7A7"/>
+        <a:srgbClr val="434343"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="535353"/>
+        <a:srgbClr val="A9A9A9"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="0076BA"/>
@@ -1016,12 +808,9 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1030,34 +819,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica Neue Medium"/>
+            <a:ea typeface="Helvetica Neue Medium"/>
+            <a:cs typeface="Helvetica Neue Medium"/>
+            <a:sym typeface="Helvetica Neue Medium"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1305,12 +1094,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:srgbClr val="FFFFFF"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1601,7 +1390,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1621,7 +1410,7 @@
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="000000"/>
+              <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -1879,742 +1668,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A2:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="12" width="16.3516" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="4" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="6" width="16.3516" style="18" customWidth="1"/>
+    <col min="7" max="8" width="16.2969" style="24" customWidth="1"/>
+    <col min="9" max="10" width="16.3516" style="25" customWidth="1"/>
+    <col min="11" max="12" width="16.3516" style="26" customWidth="1"/>
+    <col min="13" max="16384" width="16.3516" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="8">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="11"/>
     </row>
     <row r="3" ht="32.45" customHeight="1">
-      <c r="A3" t="s" s="12">
+      <c r="A3" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="13">
+      <c r="B3" t="s" s="7">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="14">
+      <c r="C3" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="15">
+      <c r="D3" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="11"/>
     </row>
     <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="16">
+      <c r="A4" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="17">
+      <c r="B4" t="s" s="11">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="18">
+      <c r="C4" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="19">
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" ht="20.2" customHeight="1">
+      <c r="A5" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11"/>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="16">
+      <c r="B5" t="s" s="11">
         <v>13</v>
       </c>
-      <c r="B5" t="s" s="17">
+      <c r="C5" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" ht="20.2" customHeight="1">
+      <c r="A6" t="s" s="10">
         <v>14</v>
       </c>
-      <c r="C5" t="s" s="18">
+      <c r="B6" t="s" s="11">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" ht="20.2" customHeight="1">
+      <c r="A7" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s" s="11">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" ht="20.2" customHeight="1">
+      <c r="A8" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s" s="11">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="11"/>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="16">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s" s="17">
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" ht="32.2" customHeight="1">
+      <c r="A9" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s" s="11">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s" s="12">
+        <v>23</v>
+      </c>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" ht="20.2" customHeight="1">
+      <c r="A10" t="s" s="10">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s" s="11">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" ht="20.2" customHeight="1">
+      <c r="A11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s" s="12">
         <v>16</v>
       </c>
-      <c r="C6" t="s" s="18">
-        <v>17</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="11"/>
-    </row>
-    <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" t="s" s="16">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s" s="17">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s" s="18">
-        <v>17</v>
-      </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11"/>
-    </row>
-    <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s" s="17">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s" s="18">
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" ht="20.2" customHeight="1">
+      <c r="A12" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s" s="11">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" ht="32.2" customHeight="1">
-      <c r="A9" t="s" s="16">
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" ht="20.2" customHeight="1">
+      <c r="A13" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s" s="11">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" ht="20.2" customHeight="1">
+      <c r="A14" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s" s="11">
         <v>22</v>
       </c>
-      <c r="B9" t="s" s="17">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s" s="18">
-        <v>24</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" t="s" s="16">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s" s="17">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s" s="18">
+      <c r="C14" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s" s="17">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s" s="18">
-        <v>17</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" ht="20.2" customHeight="1">
-      <c r="A12" t="s" s="16">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s" s="17">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s" s="18">
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" ht="20.2" customHeight="1">
+      <c r="A15" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s" s="15">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s" s="16">
         <v>11</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" ht="20.2" customHeight="1">
-      <c r="A13" t="s" s="16">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s" s="17">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s" s="18">
-        <v>11</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" ht="20.2" customHeight="1">
-      <c r="A14" t="s" s="16">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s" s="17">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s" s="18">
-        <v>11</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" ht="20.2" customHeight="1">
-      <c r="A15" t="s" s="21">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s" s="22">
+      <c r="D15" s="17"/>
+    </row>
+    <row r="17" ht="25.65" customHeight="1">
+      <c r="E17" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="C15" t="s" s="23">
-        <v>11</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="11"/>
-    </row>
-    <row r="16" ht="14.7" customHeight="1">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="11"/>
-    </row>
-    <row r="17" ht="25.65" customHeight="1">
-      <c r="A17" s="27"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" t="s" s="28">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" ht="20.45" customHeight="1">
+      <c r="E18" t="s" s="3">
         <v>34</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="11"/>
-    </row>
-    <row r="18" ht="20.45" customHeight="1">
-      <c r="A18" s="27"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="30"/>
-      <c r="E18" t="s" s="6">
+      <c r="F18" t="s" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" ht="20.45" customHeight="1">
+      <c r="E19" s="19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s" s="9">
         <v>35</v>
       </c>
-      <c r="F18" t="s" s="8">
+    </row>
+    <row r="20" ht="20.2" customHeight="1">
+      <c r="E20" s="20">
         <v>2</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="11"/>
-    </row>
-    <row r="19" ht="20.45" customHeight="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31">
+      <c r="F20" t="s" s="21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" ht="20.2" customHeight="1">
+      <c r="E21" s="20">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s" s="21">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" ht="20.2" customHeight="1">
+      <c r="E22" s="22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s" s="23">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" ht="25.65" customHeight="1">
+      <c r="G24" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" ht="20.55" customHeight="1">
+      <c r="G25" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="H25" t="s" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" ht="20.55" customHeight="1">
+      <c r="G26" s="19">
         <v>1</v>
       </c>
-      <c r="F19" t="s" s="15">
-        <v>36</v>
-      </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="11"/>
-    </row>
-    <row r="20" ht="20.2" customHeight="1">
-      <c r="A20" s="27"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="32">
+      <c r="H26" t="s" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" ht="20.3" customHeight="1">
+      <c r="G27" s="20">
         <v>2</v>
       </c>
-      <c r="F20" t="s" s="19">
-        <v>37</v>
-      </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="11"/>
-    </row>
-    <row r="21" ht="20.2" customHeight="1">
-      <c r="A21" s="27"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="32">
+      <c r="H27" t="s" s="21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" ht="20.3" customHeight="1">
+      <c r="G28" s="20">
         <v>3</v>
       </c>
-      <c r="F21" t="s" s="19">
-        <v>38</v>
-      </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="11"/>
-    </row>
-    <row r="22" ht="20.2" customHeight="1">
-      <c r="A22" s="27"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="33">
+      <c r="H28" t="s" s="21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" ht="20.3" customHeight="1">
+      <c r="G29" s="22">
         <v>4</v>
       </c>
-      <c r="F22" t="s" s="34">
-        <v>39</v>
-      </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="11"/>
-    </row>
-    <row r="23" ht="14.7" customHeight="1">
-      <c r="A23" s="27"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="11"/>
-    </row>
-    <row r="24" ht="25.65" customHeight="1">
-      <c r="A24" s="27"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" t="s" s="28">
-        <v>40</v>
-      </c>
-      <c r="H24" s="29"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="11"/>
-    </row>
-    <row r="25" ht="20.55" customHeight="1">
-      <c r="A25" s="27"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="30"/>
-      <c r="G25" t="s" s="6">
-        <v>35</v>
-      </c>
-      <c r="H25" t="s" s="8">
+      <c r="H29" t="s" s="23">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" ht="25.65" customHeight="1">
+      <c r="I31" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" ht="20.45" customHeight="1">
+      <c r="I32" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="J32" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="11"/>
-    </row>
-    <row r="26" ht="20.55" customHeight="1">
-      <c r="A26" s="27"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="31">
+    </row>
+    <row r="33" ht="20.45" customHeight="1">
+      <c r="I33" s="19">
         <v>1</v>
       </c>
-      <c r="H26" t="s" s="15">
-        <v>41</v>
-      </c>
-      <c r="I26" s="9"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="11"/>
-    </row>
-    <row r="27" ht="20.3" customHeight="1">
-      <c r="A27" s="27"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="32">
+      <c r="J33" t="s" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" ht="20.2" customHeight="1">
+      <c r="I34" s="20">
         <v>2</v>
       </c>
-      <c r="H27" t="s" s="19">
-        <v>42</v>
-      </c>
-      <c r="I27" s="9"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="11"/>
-    </row>
-    <row r="28" ht="20.3" customHeight="1">
-      <c r="A28" s="27"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="32">
+      <c r="J34" t="s" s="21">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" ht="20.2" customHeight="1">
+      <c r="I35" s="22">
         <v>3</v>
       </c>
-      <c r="H28" t="s" s="19">
-        <v>43</v>
-      </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="11"/>
-    </row>
-    <row r="29" ht="20.3" customHeight="1">
-      <c r="A29" s="27"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="33">
-        <v>4</v>
-      </c>
-      <c r="H29" t="s" s="34">
-        <v>44</v>
-      </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="11"/>
-    </row>
-    <row r="30" ht="14.7" customHeight="1">
-      <c r="A30" s="27"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="11"/>
-    </row>
-    <row r="31" ht="25.65" customHeight="1">
-      <c r="A31" s="27"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" t="s" s="28">
-        <v>45</v>
-      </c>
-      <c r="J31" s="29"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="11"/>
-    </row>
-    <row r="32" ht="20.45" customHeight="1">
-      <c r="A32" s="27"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="30"/>
-      <c r="I32" t="s" s="6">
-        <v>35</v>
-      </c>
-      <c r="J32" t="s" s="8">
+      <c r="J35" t="s" s="23">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" ht="25.65" customHeight="1">
+      <c r="K37" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" ht="20.45" customHeight="1">
+      <c r="K38" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="L38" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="K32" s="9"/>
-      <c r="L32" s="11"/>
-    </row>
-    <row r="33" ht="20.45" customHeight="1">
-      <c r="A33" s="27"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31">
+    </row>
+    <row r="39" ht="20.45" customHeight="1">
+      <c r="K39" s="19">
         <v>1</v>
       </c>
-      <c r="J33" t="s" s="15">
-        <v>46</v>
-      </c>
-      <c r="K33" s="9"/>
-      <c r="L33" s="11"/>
-    </row>
-    <row r="34" ht="20.2" customHeight="1">
-      <c r="A34" s="27"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="32">
+      <c r="L39" t="s" s="9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" ht="20.2" customHeight="1">
+      <c r="K40" s="22">
         <v>2</v>
       </c>
-      <c r="J34" t="s" s="19">
-        <v>47</v>
-      </c>
-      <c r="K34" s="9"/>
-      <c r="L34" s="11"/>
-    </row>
-    <row r="35" ht="20.2" customHeight="1">
-      <c r="A35" s="27"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="33">
-        <v>3</v>
-      </c>
-      <c r="J35" t="s" s="34">
-        <v>48</v>
-      </c>
-      <c r="K35" s="9"/>
-      <c r="L35" s="11"/>
-    </row>
-    <row r="36" ht="14.7" customHeight="1">
-      <c r="A36" s="27"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="11"/>
-    </row>
-    <row r="37" ht="25.65" customHeight="1">
-      <c r="A37" s="27"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" t="s" s="28">
-        <v>49</v>
-      </c>
-      <c r="L37" s="35"/>
-    </row>
-    <row r="38" ht="20.45" customHeight="1">
-      <c r="A38" s="27"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="30"/>
-      <c r="K38" t="s" s="6">
-        <v>35</v>
-      </c>
-      <c r="L38" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" ht="20.45" customHeight="1">
-      <c r="A39" s="27"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="31">
-        <v>1</v>
-      </c>
-      <c r="L39" t="s" s="15">
+      <c r="L40" t="s" s="23">
         <v>50</v>
-      </c>
-    </row>
-    <row r="40" ht="20.2" customHeight="1">
-      <c r="A40" s="36"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="33">
-        <v>2</v>
-      </c>
-      <c r="L40" t="s" s="34">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2628,7 +2035,7 @@
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;KFEFFFE&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>